<commit_message>
New changes in doc
</commit_message>
<xml_diff>
--- a/Documentation/5.- Gestión del Proyecto/5.3.- Métricas del Proceso/1.- Cálculo de los puntos de función.xlsx
+++ b/Documentation/5.- Gestión del Proyecto/5.3.- Métricas del Proceso/1.- Cálculo de los puntos de función.xlsx
@@ -11,15 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>Categoria</t>
   </si>
   <si>
     <t>Nombre punto de funcion</t>
-  </si>
-  <si>
-    <t>Dificultad</t>
   </si>
   <si>
     <t>Cuenta_total</t>
@@ -563,10 +560,9 @@
     <col min="1" customWidth="1" max="1" width="21.29"/>
     <col min="2" customWidth="1" max="2" width="71.14"/>
     <col min="3" customWidth="1" max="3" width="23.14"/>
-    <col min="4" customWidth="1" max="4" width="12.0"/>
-    <col min="5" customWidth="1" max="5" width="35.57"/>
-    <col min="6" customWidth="1" max="6" width="31.57"/>
-    <col min="7" customWidth="1" max="7" width="54.57"/>
+    <col min="4" customWidth="1" max="4" width="35.57"/>
+    <col min="5" customWidth="1" max="5" width="31.57"/>
+    <col min="6" customWidth="1" max="6" width="54.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -579,1041 +575,905 @@
       <c t="s" s="13" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="4" r="D1">
+      <c t="s" s="13" r="D1">
         <v>3</v>
       </c>
       <c t="s" s="13" r="E1">
         <v>4</v>
       </c>
-      <c t="s" s="13" r="F1">
-        <v>5</v>
-      </c>
-      <c s="1" r="G1"/>
+      <c s="1" r="F1"/>
     </row>
     <row r="2">
       <c t="s" s="6" r="A2">
+        <v>5</v>
+      </c>
+      <c t="s" s="6" r="B2">
         <v>6</v>
-      </c>
-      <c t="s" s="6" r="B2">
-        <v>7</v>
       </c>
       <c s="6" r="C2">
         <v>1</v>
       </c>
       <c s="6" r="D2">
-        <v>1</v>
+        <f>SUM(C2:C50)</f>
+        <v>158</v>
       </c>
       <c s="6" r="E2">
-        <f>SUM(C2:C50)</f>
-        <v>158</v>
-      </c>
-      <c s="6" r="F2">
-        <f>C2*(0.65+(0.01*E2))</f>
+        <f>C2*(0.65+(0.01*D2))</f>
         <v>2.23</v>
       </c>
-      <c s="1" r="G2"/>
+      <c s="1" r="F2"/>
     </row>
     <row r="3">
       <c t="s" s="6" r="A3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c t="s" s="6" r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c s="6" r="C3">
         <v>2</v>
       </c>
       <c s="6" r="D3">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E3">
-        <v>158</v>
-      </c>
-      <c s="6" r="F3">
-        <f>C3*(0.65+(0.01*E3))</f>
+        <f>C3*(0.65+(0.01*D3))</f>
         <v>4.46</v>
       </c>
-      <c s="1" r="G3"/>
+      <c s="1" r="F3"/>
     </row>
     <row r="4">
       <c t="s" s="6" r="A4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c t="s" s="6" r="B4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c s="6" r="C4">
         <v>2</v>
       </c>
       <c s="6" r="D4">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E4">
-        <v>158</v>
-      </c>
-      <c s="6" r="F4">
-        <f>C4*(0.65+(0.01*E4))</f>
+        <f>C4*(0.65+(0.01*D4))</f>
         <v>4.46</v>
       </c>
-      <c s="1" r="G4"/>
+      <c s="1" r="F4"/>
     </row>
     <row r="5">
       <c t="s" s="6" r="A5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c t="s" s="6" r="B5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c s="6" r="C5">
         <v>4</v>
       </c>
       <c s="6" r="D5">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E5">
-        <v>158</v>
-      </c>
-      <c s="6" r="F5">
-        <f>C5*(0.65+(0.01*E5))</f>
+        <f>C5*(0.65+(0.01*D5))</f>
         <v>8.92</v>
       </c>
-      <c s="1" r="G5"/>
+      <c s="1" r="F5"/>
     </row>
     <row r="6">
       <c t="s" s="6" r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c t="s" s="6" r="B6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c s="6" r="C6">
         <v>4</v>
       </c>
       <c s="6" r="D6">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E6">
-        <v>158</v>
-      </c>
-      <c s="6" r="F6">
-        <f>C6*(0.65+(0.01*E6))</f>
+        <f>C6*(0.65+(0.01*D6))</f>
         <v>8.92</v>
       </c>
-      <c s="1" r="G6"/>
+      <c s="1" r="F6"/>
     </row>
     <row r="7">
       <c t="s" s="6" r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c t="s" s="6" r="B7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c s="6" r="C7">
         <v>2</v>
       </c>
       <c s="6" r="D7">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E7">
-        <v>158</v>
-      </c>
-      <c s="6" r="F7">
-        <f>C7*(0.65+(0.01*E7))</f>
+        <f>C7*(0.65+(0.01*D7))</f>
         <v>4.46</v>
       </c>
-      <c s="1" r="G7"/>
+      <c s="1" r="F7"/>
     </row>
     <row r="8">
       <c t="s" s="6" r="A8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c t="s" s="6" r="B8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c s="6" r="C8">
         <v>2</v>
       </c>
       <c s="6" r="D8">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E8">
-        <v>158</v>
-      </c>
-      <c s="6" r="F8">
-        <f>C8*(0.65+(0.01*E8))</f>
+        <f>C8*(0.65+(0.01*D8))</f>
         <v>4.46</v>
       </c>
-      <c s="1" r="G8"/>
+      <c s="1" r="F8"/>
     </row>
     <row r="9">
       <c t="s" s="6" r="A9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c t="s" s="6" r="B9">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c s="6" r="C9">
         <v>4</v>
       </c>
       <c s="6" r="D9">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E9">
-        <v>158</v>
-      </c>
-      <c s="6" r="F9">
-        <f>C9*(0.65+(0.01*E9))</f>
+        <f>C9*(0.65+(0.01*D9))</f>
         <v>8.92</v>
       </c>
-      <c s="1" r="G9"/>
+      <c s="1" r="F9"/>
     </row>
     <row r="10">
       <c s="6" r="A10"/>
       <c s="6" r="B10"/>
       <c s="6" r="C10"/>
-      <c s="6" r="D10"/>
+      <c s="6" r="D10">
+        <v>158</v>
+      </c>
       <c s="6" r="E10">
-        <v>158</v>
-      </c>
-      <c s="6" r="F10">
-        <f>C10*(0.65+(0.01*E10))</f>
+        <f>C10*(0.65+(0.01*D10))</f>
         <v>0</v>
       </c>
-      <c t="s" s="5" r="G10">
-        <v>15</v>
+      <c t="s" s="5" r="F10">
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="6" r="A11">
+        <v>15</v>
+      </c>
+      <c t="s" s="6" r="B11">
         <v>16</v>
-      </c>
-      <c t="s" s="6" r="B11">
-        <v>17</v>
       </c>
       <c s="6" r="C11">
         <v>6</v>
       </c>
       <c s="6" r="D11">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E11">
-        <v>158</v>
-      </c>
-      <c s="6" r="F11">
-        <f>C11*(0.65+(0.01*E11))</f>
+        <f>C11*(0.65+(0.01*D11))</f>
         <v>13.38</v>
       </c>
-      <c s="1" r="G11"/>
+      <c s="1" r="F11"/>
     </row>
     <row r="12">
       <c t="s" s="6" r="A12">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c t="s" s="6" r="B12">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c s="6" r="C12">
         <v>6</v>
       </c>
       <c s="6" r="D12">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E12">
-        <v>158</v>
-      </c>
-      <c s="6" r="F12">
-        <f>C12*(0.65+(0.01*E12))</f>
+        <f>C12*(0.65+(0.01*D12))</f>
         <v>13.38</v>
       </c>
-      <c s="1" r="G12"/>
+      <c s="1" r="F12"/>
     </row>
     <row r="13">
       <c t="s" s="6" r="A13">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c t="s" s="6" r="B13">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c s="6" r="C13">
         <v>3</v>
       </c>
       <c s="6" r="D13">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E13">
-        <v>158</v>
-      </c>
-      <c s="6" r="F13">
-        <f>C13*(0.65+(0.01*E13))</f>
+        <f>C13*(0.65+(0.01*D13))</f>
         <v>6.69</v>
       </c>
-      <c s="1" r="G13"/>
+      <c s="1" r="F13"/>
     </row>
     <row r="14">
       <c t="s" s="6" r="A14">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c t="s" s="6" r="B14">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c s="6" r="C14">
         <v>3</v>
       </c>
       <c s="6" r="D14">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E14">
-        <v>158</v>
-      </c>
-      <c s="6" r="F14">
-        <f>C14*(0.65+(0.01*E14))</f>
+        <f>C14*(0.65+(0.01*D14))</f>
         <v>6.69</v>
       </c>
-      <c s="1" r="G14"/>
+      <c s="1" r="F14"/>
     </row>
     <row r="15">
       <c t="s" s="6" r="A15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c t="s" s="6" r="B15">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c s="6" r="C15">
         <v>3</v>
       </c>
       <c s="6" r="D15">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E15">
-        <v>158</v>
-      </c>
-      <c s="6" r="F15">
-        <f>C15*(0.65+(0.01*E15))</f>
+        <f>C15*(0.65+(0.01*D15))</f>
         <v>6.69</v>
       </c>
-      <c s="1" r="G15"/>
+      <c s="1" r="F15"/>
     </row>
     <row r="16">
       <c t="s" s="6" r="A16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c t="s" s="6" r="B16">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c s="6" r="C16">
         <v>4</v>
       </c>
       <c s="6" r="D16">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E16">
-        <v>158</v>
-      </c>
-      <c s="6" r="F16">
-        <f>C16*(0.65+(0.01*E16))</f>
+        <f>C16*(0.65+(0.01*D16))</f>
         <v>8.92</v>
       </c>
-      <c s="1" r="G16"/>
+      <c s="1" r="F16"/>
     </row>
     <row r="17">
       <c t="s" s="6" r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c t="s" s="6" r="B17">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c s="6" r="C17">
         <v>5</v>
       </c>
       <c s="6" r="D17">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E17">
-        <v>158</v>
-      </c>
-      <c s="6" r="F17">
-        <f>C17*(0.65+(0.01*E17))</f>
+        <f>C17*(0.65+(0.01*D17))</f>
         <v>11.15</v>
       </c>
-      <c s="1" r="G17"/>
+      <c s="1" r="F17"/>
     </row>
     <row r="18">
       <c t="s" s="6" r="A18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c t="s" s="6" r="B18">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c s="6" r="C18">
         <v>5</v>
       </c>
       <c s="6" r="D18">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E18">
-        <v>158</v>
-      </c>
-      <c s="6" r="F18">
-        <f>C18*(0.65+(0.01*E18))</f>
+        <f>C18*(0.65+(0.01*D18))</f>
         <v>11.15</v>
       </c>
-      <c s="1" r="G18"/>
+      <c s="1" r="F18"/>
     </row>
     <row r="19">
       <c t="s" s="6" r="A19">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c t="s" s="6" r="B19">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c s="6" r="C19">
         <v>3</v>
       </c>
       <c s="6" r="D19">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E19">
-        <v>158</v>
-      </c>
-      <c s="6" r="F19">
-        <f>C19*(0.65+(0.01*E19))</f>
+        <f>C19*(0.65+(0.01*D19))</f>
         <v>6.69</v>
       </c>
-      <c s="1" r="G19"/>
+      <c s="1" r="F19"/>
     </row>
     <row r="20">
       <c s="6" r="A20"/>
       <c s="6" r="B20"/>
       <c s="6" r="C20"/>
-      <c s="6" r="D20"/>
+      <c s="6" r="D20">
+        <v>158</v>
+      </c>
       <c s="6" r="E20">
-        <v>158</v>
-      </c>
-      <c s="6" r="F20">
-        <f>C20*(0.65+(0.01*E20))</f>
+        <f>C20*(0.65+(0.01*D20))</f>
         <v>0</v>
       </c>
-      <c s="1" r="G20"/>
+      <c s="1" r="F20"/>
     </row>
     <row r="21">
       <c s="6" r="A21"/>
       <c s="6" r="B21"/>
       <c s="6" r="C21"/>
-      <c s="6" r="D21"/>
+      <c s="6" r="D21">
+        <v>158</v>
+      </c>
       <c s="6" r="E21">
-        <v>158</v>
-      </c>
-      <c s="6" r="F21">
-        <f>C21*(0.65+(0.01*E21))</f>
+        <f>C21*(0.65+(0.01*D21))</f>
         <v>0</v>
       </c>
-      <c s="1" r="G21"/>
+      <c s="1" r="F21"/>
     </row>
     <row r="22">
       <c t="s" s="6" r="A22">
+        <v>25</v>
+      </c>
+      <c t="s" s="6" r="B22">
         <v>26</v>
-      </c>
-      <c t="s" s="6" r="B22">
-        <v>27</v>
       </c>
       <c s="6" r="C22">
         <v>3</v>
       </c>
       <c s="6" r="D22">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E22">
-        <v>158</v>
-      </c>
-      <c s="6" r="F22">
-        <f>C22*(0.65+(0.01*E22))</f>
+        <f>C22*(0.65+(0.01*D22))</f>
         <v>6.69</v>
       </c>
-      <c s="1" r="G22"/>
+      <c s="1" r="F22"/>
     </row>
     <row r="23">
       <c t="s" s="6" r="A23">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c t="s" s="6" r="B23">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c s="6" r="C23">
         <v>6</v>
       </c>
       <c s="6" r="D23">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E23">
-        <v>158</v>
-      </c>
-      <c s="6" r="F23">
-        <f>C23*(0.65+(0.01*E23))</f>
+        <f>C23*(0.65+(0.01*D23))</f>
         <v>13.38</v>
       </c>
-      <c s="1" r="G23"/>
+      <c s="1" r="F23"/>
     </row>
     <row r="24">
       <c t="s" s="6" r="A24">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c t="s" s="6" r="B24">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c s="6" r="C24">
         <v>4</v>
       </c>
       <c s="6" r="D24">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E24">
-        <v>158</v>
-      </c>
-      <c s="6" r="F24">
-        <f>C24*(0.65+(0.01*E24))</f>
+        <f>C24*(0.65+(0.01*D24))</f>
         <v>8.92</v>
       </c>
-      <c s="1" r="G24"/>
+      <c s="1" r="F24"/>
     </row>
     <row r="25">
       <c s="6" r="A25"/>
       <c s="6" r="B25"/>
       <c s="6" r="C25"/>
-      <c s="6" r="D25"/>
+      <c s="6" r="D25">
+        <v>158</v>
+      </c>
       <c s="6" r="E25">
-        <v>158</v>
-      </c>
-      <c s="6" r="F25">
-        <f>C25*(0.65+(0.01*E25))</f>
+        <f>C25*(0.65+(0.01*D25))</f>
         <v>0</v>
       </c>
-      <c s="1" r="G25"/>
+      <c s="1" r="F25"/>
     </row>
     <row r="26">
       <c t="s" s="6" r="A26">
+        <v>29</v>
+      </c>
+      <c t="s" s="6" r="B26">
         <v>30</v>
-      </c>
-      <c t="s" s="6" r="B26">
-        <v>31</v>
       </c>
       <c s="6" r="C26">
         <v>5</v>
       </c>
       <c s="6" r="D26">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E26">
-        <v>158</v>
-      </c>
-      <c s="6" r="F26">
-        <f>C26*(0.65+(0.01*E26))</f>
+        <f>C26*(0.65+(0.01*D26))</f>
         <v>11.15</v>
       </c>
-      <c s="1" r="G26"/>
+      <c s="1" r="F26"/>
     </row>
     <row r="27">
       <c t="s" s="6" r="A27">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c t="s" s="6" r="B27">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c s="6" r="C27">
         <v>3</v>
       </c>
       <c s="6" r="D27">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E27">
-        <v>158</v>
-      </c>
-      <c s="6" r="F27">
-        <f>C27*(0.65+(0.01*E27))</f>
+        <f>C27*(0.65+(0.01*D27))</f>
         <v>6.69</v>
       </c>
-      <c s="1" r="G27"/>
+      <c s="1" r="F27"/>
     </row>
     <row r="28">
       <c t="s" s="6" r="A28">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c t="s" s="6" r="B28">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c s="6" r="C28">
         <v>7</v>
       </c>
       <c s="6" r="D28">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E28">
-        <v>158</v>
-      </c>
-      <c s="6" r="F28">
-        <f>C28*(0.65+(0.01*E28))</f>
+        <f>C28*(0.65+(0.01*D28))</f>
         <v>15.61</v>
       </c>
-      <c s="1" r="G28"/>
+      <c s="1" r="F28"/>
     </row>
     <row r="29">
       <c t="s" s="6" r="A29">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c t="s" s="6" r="B29">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c s="6" r="C29">
         <v>9</v>
       </c>
       <c s="6" r="D29">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E29">
-        <v>158</v>
-      </c>
-      <c s="6" r="F29">
-        <f>C29*(0.65+(0.01*E29))</f>
+        <f>C29*(0.65+(0.01*D29))</f>
         <v>20.07</v>
       </c>
-      <c s="1" r="G29"/>
+      <c s="1" r="F29"/>
     </row>
     <row r="30">
       <c t="s" s="6" r="A30">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c t="s" s="6" r="B30">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c s="6" r="C30">
         <v>3</v>
       </c>
       <c s="6" r="D30">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E30">
-        <v>158</v>
-      </c>
-      <c s="6" r="F30">
-        <f>C30*(0.65+(0.01*E30))</f>
+        <f>C30*(0.65+(0.01*D30))</f>
         <v>6.69</v>
       </c>
-      <c s="1" r="G30"/>
+      <c s="1" r="F30"/>
     </row>
     <row r="31">
       <c t="s" s="6" r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c t="s" s="6" r="B31">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c s="6" r="C31">
         <v>8</v>
       </c>
       <c s="6" r="D31">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E31">
-        <v>158</v>
-      </c>
-      <c s="6" r="F31">
-        <f>C31*(0.65+(0.01*E31))</f>
+        <f>C31*(0.65+(0.01*D31))</f>
         <v>17.84</v>
       </c>
-      <c s="1" r="G31"/>
+      <c s="1" r="F31"/>
     </row>
     <row r="32">
       <c s="6" r="A32"/>
       <c s="6" r="B32"/>
       <c s="6" r="C32"/>
-      <c s="6" r="D32"/>
+      <c s="6" r="D32">
+        <v>158</v>
+      </c>
       <c s="6" r="E32">
-        <v>158</v>
-      </c>
-      <c s="6" r="F32">
-        <f>C32*(0.65+(0.01*E32))</f>
+        <f>C32*(0.65+(0.01*D32))</f>
         <v>0</v>
       </c>
-      <c s="1" r="G32"/>
+      <c s="1" r="F32"/>
     </row>
     <row r="33">
       <c t="s" s="6" r="A33">
+        <v>36</v>
+      </c>
+      <c t="s" s="6" r="B33">
         <v>37</v>
-      </c>
-      <c t="s" s="6" r="B33">
-        <v>38</v>
       </c>
       <c s="6" r="C33">
         <v>6</v>
       </c>
       <c s="6" r="D33">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E33">
-        <v>158</v>
-      </c>
-      <c s="6" r="F33">
-        <f>C33*(0.65+(0.01*E33))</f>
+        <f>C33*(0.65+(0.01*D33))</f>
         <v>13.38</v>
       </c>
-      <c s="1" r="G33"/>
+      <c s="1" r="F33"/>
     </row>
     <row r="34">
       <c t="s" s="6" r="A34">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c t="s" s="6" r="B34">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c s="6" r="C34">
         <v>6</v>
       </c>
       <c s="6" r="D34">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E34">
-        <v>158</v>
-      </c>
-      <c s="6" r="F34">
-        <f>C34*(0.65+(0.01*E34))</f>
+        <f>C34*(0.65+(0.01*D34))</f>
         <v>13.38</v>
       </c>
-      <c s="1" r="G34"/>
+      <c s="1" r="F34"/>
     </row>
     <row r="35">
       <c t="s" s="6" r="A35">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c t="s" s="6" r="B35">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c s="6" r="C35">
         <v>3</v>
       </c>
       <c s="6" r="D35">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E35">
-        <v>158</v>
-      </c>
-      <c s="6" r="F35">
-        <f>C35*(0.65+(0.01*E35))</f>
+        <f>C35*(0.65+(0.01*D35))</f>
         <v>6.69</v>
       </c>
-      <c s="1" r="G35"/>
+      <c s="1" r="F35"/>
     </row>
     <row r="36">
       <c t="s" s="6" r="A36">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c t="s" s="6" r="B36">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c s="6" r="C36">
         <v>2</v>
       </c>
       <c s="6" r="D36">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E36">
-        <v>158</v>
-      </c>
-      <c s="6" r="F36">
-        <f>C36*(0.65+(0.01*E36))</f>
+        <f>C36*(0.65+(0.01*D36))</f>
         <v>4.46</v>
       </c>
-      <c s="1" r="G36"/>
+      <c s="1" r="F36"/>
     </row>
     <row r="37">
       <c s="6" r="A37"/>
       <c s="6" r="B37"/>
       <c s="6" r="C37"/>
-      <c s="6" r="D37"/>
+      <c s="6" r="D37">
+        <v>158</v>
+      </c>
       <c s="6" r="E37">
-        <v>158</v>
-      </c>
-      <c s="6" r="F37">
-        <f>C37*(0.65+(0.01*E37))</f>
+        <f>C37*(0.65+(0.01*D37))</f>
         <v>0</v>
       </c>
-      <c s="1" r="G37"/>
+      <c s="1" r="F37"/>
     </row>
     <row r="38">
       <c t="s" s="6" r="A38">
+        <v>41</v>
+      </c>
+      <c t="s" s="6" r="B38">
         <v>42</v>
-      </c>
-      <c t="s" s="6" r="B38">
-        <v>43</v>
       </c>
       <c s="6" r="C38">
         <v>5</v>
       </c>
       <c s="6" r="D38">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E38">
-        <v>158</v>
-      </c>
-      <c s="6" r="F38">
-        <f>C38*(0.65+(0.01*E38))</f>
+        <f>C38*(0.65+(0.01*D38))</f>
         <v>11.15</v>
       </c>
-      <c s="1" r="G38"/>
+      <c s="1" r="F38"/>
     </row>
     <row r="39">
       <c t="s" s="6" r="A39">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c t="s" s="6" r="B39">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c s="6" r="C39">
         <v>1</v>
       </c>
       <c s="6" r="D39">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E39">
-        <v>158</v>
-      </c>
-      <c s="6" r="F39">
-        <f>C39*(0.65+(0.01*E39))</f>
+        <f>C39*(0.65+(0.01*D39))</f>
         <v>2.23</v>
       </c>
-      <c s="1" r="G39"/>
+      <c s="1" r="F39"/>
     </row>
     <row r="40">
       <c t="s" s="6" r="A40">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c t="s" s="6" r="B40">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c s="6" r="C40">
         <v>1</v>
       </c>
       <c s="6" r="D40">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E40">
-        <v>158</v>
-      </c>
-      <c s="6" r="F40">
-        <f>C40*(0.65+(0.01*E40))</f>
+        <f>C40*(0.65+(0.01*D40))</f>
         <v>2.23</v>
       </c>
-      <c s="1" r="G40"/>
+      <c s="1" r="F40"/>
     </row>
     <row r="41">
       <c t="s" s="6" r="A41">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c t="s" s="6" r="B41">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c s="6" r="C41">
         <v>1</v>
       </c>
       <c s="6" r="D41">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E41">
-        <v>158</v>
-      </c>
-      <c s="6" r="F41">
-        <f>C41*(0.65+(0.01*E41))</f>
+        <f>C41*(0.65+(0.01*D41))</f>
         <v>2.23</v>
       </c>
-      <c s="1" r="G41"/>
+      <c s="1" r="F41"/>
     </row>
     <row r="42">
       <c t="s" s="6" r="A42">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c t="s" s="6" r="B42">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c s="6" r="C42">
         <v>4</v>
       </c>
       <c s="6" r="D42">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E42">
-        <v>158</v>
-      </c>
-      <c s="6" r="F42">
-        <f>C42*(0.65+(0.01*E42))</f>
+        <f>C42*(0.65+(0.01*D42))</f>
         <v>8.92</v>
       </c>
-      <c s="1" r="G42"/>
+      <c s="1" r="F42"/>
     </row>
     <row r="43">
       <c t="s" s="6" r="A43">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c t="s" s="6" r="B43">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c s="6" r="C43">
         <v>6</v>
       </c>
       <c s="6" r="D43">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E43">
-        <v>158</v>
-      </c>
-      <c s="6" r="F43">
-        <f>C43*(0.65+(0.01*E43))</f>
+        <f>C43*(0.65+(0.01*D43))</f>
         <v>13.38</v>
       </c>
-      <c s="1" r="G43"/>
+      <c s="1" r="F43"/>
     </row>
     <row r="44">
       <c t="s" s="6" r="A44">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c t="s" s="6" r="B44">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c s="6" r="C44">
         <v>1</v>
       </c>
       <c s="6" r="D44">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E44">
-        <v>158</v>
-      </c>
-      <c s="6" r="F44">
-        <f>C44*(0.65+(0.01*E44))</f>
+        <f>C44*(0.65+(0.01*D44))</f>
         <v>2.23</v>
       </c>
-      <c s="1" r="G44"/>
+      <c s="1" r="F44"/>
     </row>
     <row r="45">
       <c s="6" r="A45"/>
       <c s="6" r="B45"/>
       <c s="6" r="C45"/>
-      <c s="6" r="D45"/>
+      <c s="6" r="D45">
+        <v>158</v>
+      </c>
       <c s="6" r="E45">
-        <v>158</v>
-      </c>
-      <c s="6" r="F45">
-        <f>C45*(0.65+(0.01*E45))</f>
+        <f>C45*(0.65+(0.01*D45))</f>
         <v>0</v>
       </c>
-      <c s="1" r="G45"/>
+      <c s="1" r="F45"/>
     </row>
     <row r="46">
       <c t="s" s="6" r="A46">
+        <v>49</v>
+      </c>
+      <c t="s" s="6" r="B46">
         <v>50</v>
-      </c>
-      <c t="s" s="6" r="B46">
-        <v>51</v>
       </c>
       <c s="6" r="C46">
         <v>3</v>
       </c>
       <c s="6" r="D46">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E46">
-        <v>158</v>
-      </c>
-      <c s="6" r="F46">
-        <f>C46*(0.65+(0.01*E46))</f>
+        <f>C46*(0.65+(0.01*D46))</f>
         <v>6.69</v>
       </c>
-      <c s="1" r="G46"/>
+      <c s="1" r="F46"/>
     </row>
     <row r="47">
       <c t="s" s="6" r="A47">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c t="s" s="6" r="B47">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c s="6" r="C47">
         <v>2</v>
       </c>
       <c s="6" r="D47">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E47">
-        <v>158</v>
-      </c>
-      <c s="6" r="F47">
-        <f>C47*(0.65+(0.01*E47))</f>
+        <f>C47*(0.65+(0.01*D47))</f>
         <v>4.46</v>
       </c>
-      <c s="1" r="G47"/>
+      <c s="1" r="F47"/>
     </row>
     <row r="48">
       <c t="s" s="6" r="A48">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c t="s" s="6" r="B48">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c s="6" r="C48">
         <v>4</v>
       </c>
       <c s="6" r="D48">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E48">
-        <v>158</v>
-      </c>
-      <c s="6" r="F48">
-        <f>C48*(0.65+(0.01*E48))</f>
+        <f>C48*(0.65+(0.01*D48))</f>
         <v>8.92</v>
       </c>
-      <c s="1" r="G48"/>
+      <c s="1" r="F48"/>
     </row>
     <row r="49">
       <c t="s" s="6" r="A49">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c t="s" s="6" r="B49">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c s="6" r="C49">
         <v>4</v>
       </c>
       <c s="6" r="D49">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E49">
-        <v>158</v>
-      </c>
-      <c s="6" r="F49">
-        <f>C49*(0.65+(0.01*E49))</f>
+        <f>C49*(0.65+(0.01*D49))</f>
         <v>8.92</v>
       </c>
-      <c s="1" r="G49"/>
+      <c s="1" r="F49"/>
     </row>
     <row r="50">
       <c t="s" s="6" r="A50">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c t="s" s="6" r="B50">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c s="6" r="C50">
         <v>2</v>
       </c>
       <c s="6" r="D50">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c s="6" r="E50">
-        <v>158</v>
-      </c>
-      <c s="6" r="F50">
-        <f>C50*(0.65+(0.01*E50))</f>
+        <f>C50*(0.65+(0.01*D50))</f>
         <v>4.46</v>
       </c>
-      <c s="1" r="G50"/>
+      <c s="1" r="F50"/>
     </row>
     <row r="51">
       <c s="9" r="A51"/>
@@ -1621,107 +1481,102 @@
       <c s="9" r="C51"/>
       <c s="9" r="D51"/>
       <c s="9" r="E51"/>
-      <c s="9" r="F51"/>
     </row>
     <row r="52">
       <c t="s" s="7" r="A52">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c s="7" r="B52"/>
       <c s="7" r="C52">
         <f>SUM(C2:C50)</f>
         <v>158</v>
       </c>
-      <c s="7" r="D52">
-        <f>SUM(D2:D50)</f>
-        <v>42</v>
-      </c>
-      <c s="7" r="E52"/>
-      <c s="7" r="F52">
-        <f>SUM(F2:F50)</f>
+      <c s="7" r="D52"/>
+      <c s="7" r="E52">
+        <f>SUM(E2:E50)</f>
         <v>352.34</v>
       </c>
-      <c t="s" s="14" r="G52">
+      <c t="s" s="14" r="F52">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53">
+      <c s="2" r="E53"/>
+      <c s="14" r="F53"/>
+    </row>
+    <row r="54">
+      <c s="12" r="E54"/>
+      <c s="12" r="F54"/>
+    </row>
+    <row r="55">
+      <c s="8" r="D55"/>
+      <c s="3" r="E55">
+        <v>0.2727</v>
+      </c>
+      <c t="s" s="11" r="F55">
         <v>57</v>
       </c>
-    </row>
-    <row r="53">
-      <c s="2" r="F53"/>
-      <c s="14" r="G53"/>
-    </row>
-    <row r="54">
-      <c s="12" r="F54"/>
-      <c s="12" r="G54"/>
-    </row>
-    <row r="55">
-      <c s="8" r="E55"/>
-      <c s="3" r="F55">
-        <v>0.2727</v>
-      </c>
-      <c t="s" s="11" r="G55">
+      <c s="1" r="G55"/>
+    </row>
+    <row r="56">
+      <c s="8" r="D56"/>
+      <c s="3" r="E56">
+        <v>0.3699</v>
+      </c>
+      <c t="s" s="11" r="F56">
         <v>58</v>
       </c>
-      <c s="1" r="H55"/>
-    </row>
-    <row r="56">
-      <c s="8" r="E56"/>
-      <c s="3" r="F56">
-        <v>0.3699</v>
-      </c>
-      <c t="s" s="11" r="G56">
+      <c s="1" r="G56"/>
+    </row>
+    <row r="57">
+      <c s="8" r="D57"/>
+      <c s="3" r="E57">
+        <v>0.5899</v>
+      </c>
+      <c t="s" s="11" r="F57">
         <v>59</v>
       </c>
-      <c s="1" r="H56"/>
-    </row>
-    <row r="57">
-      <c s="8" r="E57"/>
-      <c s="3" r="F57">
-        <v>0.5899</v>
-      </c>
-      <c t="s" s="11" r="G57">
-        <v>60</v>
-      </c>
-      <c s="1" r="H57"/>
+      <c s="1" r="G57"/>
     </row>
     <row r="58">
-      <c s="8" r="E58"/>
-      <c s="3" r="F58">
+      <c s="8" r="D58"/>
+      <c s="3" r="E58">
         <v>1</v>
       </c>
-      <c t="s" s="11" r="G58">
-        <v>60</v>
-      </c>
-      <c s="1" r="H58"/>
+      <c t="s" s="11" r="F58">
+        <v>59</v>
+      </c>
+      <c s="1" r="G58"/>
     </row>
     <row r="59">
+      <c s="9" r="E59"/>
       <c s="9" r="F59"/>
-      <c s="9" r="G59"/>
     </row>
     <row r="62">
       <c t="s" s="15" r="A62">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c s="12" r="B62"/>
       <c s="12" r="C62"/>
     </row>
     <row r="63">
       <c t="s" s="13" r="A63">
+        <v>61</v>
+      </c>
+      <c t="s" s="13" r="B63">
         <v>62</v>
       </c>
-      <c t="s" s="13" r="B63">
+      <c t="s" s="13" r="C63">
         <v>63</v>
-      </c>
-      <c t="s" s="13" r="C63">
-        <v>64</v>
       </c>
       <c s="1" r="D63"/>
     </row>
     <row r="64">
       <c t="s" s="6" r="A64">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c s="6" r="B64">
-        <f>SUM(F22:F24)</f>
+        <f>SUM(E22:E24)</f>
         <v>28.99</v>
       </c>
       <c s="6" r="C64">
@@ -1732,10 +1587,10 @@
     </row>
     <row r="65">
       <c t="s" s="6" r="A65">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c s="6" r="B65">
-        <f>SUM(F2:F9)</f>
+        <f>SUM(E2:E9)</f>
         <v>46.83</v>
       </c>
       <c s="6" r="C65">
@@ -1746,10 +1601,10 @@
     </row>
     <row r="66">
       <c t="s" s="6" r="A66">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c s="6" r="B66">
-        <f>SUM(F11:F19)</f>
+        <f>SUM(E11:E19)</f>
         <v>84.74</v>
       </c>
       <c s="10" r="C66">
@@ -1760,10 +1615,10 @@
     </row>
     <row r="67">
       <c t="s" s="6" r="A67">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c s="6" r="B67">
-        <f>SUM(F38:F50)</f>
+        <f>SUM(E38:E50)</f>
         <v>75.82</v>
       </c>
       <c s="10" r="C67">
@@ -1774,10 +1629,10 @@
     </row>
     <row r="68">
       <c t="s" s="6" r="A68">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c s="6" r="B68">
-        <f>SUM(F26:F31)</f>
+        <f>SUM(E26:E31)</f>
         <v>78.05</v>
       </c>
       <c s="10" r="C68">
@@ -1792,8 +1647,8 @@
       <c s="9" r="C69"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F24">
-    <sortState ref="A1:F24"/>
+  <autoFilter ref="A1:E24">
+    <sortState ref="A1:E24"/>
   </autoFilter>
 </worksheet>
 </file>
</xml_diff>